<commit_message>
msg correta conforme tainá
</commit_message>
<xml_diff>
--- a/mensagens.xlsx
+++ b/mensagens.xlsx
@@ -452,7 +452,9 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>Olá A CRUZ DA SILVA COLCHOES E ESTOFADOS,
-Segue o resumo dos seus débitos consultados no dia 30/01/25:
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
 **Referente a 08/2024:**
   - Departamento Pessoal: R$ 644.04
 **Referente a 09/2024:**
@@ -465,8 +467,14 @@
   - Departamento Pessoal: R$ 543.07
 **Referente a 2024:**
   - Departamento Pessoal: R$ 99.60
-A CRUZ DA SILVA COLCHOES E ESTOFADOS, com base em consulta no dia 30/01/25, 
-Você tem os processos 90.4.25.000350-37, 90.4.25.000493-30, 90.4.25.000521-28 em 'ATIVA NAO AJUIZAVEL EM PROCESSO DE NEGOCIACAO NO SISPAR'.</t>
+A empresa possui os seguintes débitos referente a parcelamentos: 
+ATIVA NAO AJUIZAVEL EM PROCESSO DE NEGOCIACAO NO SISPAR'.
+Os valores informados são válidos na data de envio deste e-mail (03/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
         </is>
       </c>
     </row>
@@ -477,7 +485,9 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>Olá ADIALA MOVEIS EXCLUSIVOS LTDA,
-Segue o resumo dos seus débitos consultados no dia 30/01/25:
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
 **Referente a 01/2024:**
   - Departamento Pessoal: R$ 975.72
 **Referente a 02/2024:**
@@ -502,23 +512,33 @@
   - Departamento Pessoal: R$ 41.70
 **Referente a 12/2023:**
   - Departamento Pessoal: R$ 981.75
-ADIALA MOVEIS EXCLUSIVOS, com base em consulta no dia 30/01/25, 
-Você tem os processos 18433540-0, 19672009-5 em '000520 - INSCRICAO DE CREDITO EM DIVIDA ATIVA'.
-Você tem os processos 16454705-3, 18373640-0 em '000797 - PARCELAMENTO RESCINDIDO'.
-Você tem os processos 90.4.20.003200-34, 90.4.20.025081-70, 90.4.21.002594-85, 90.4.23.059467-00 em 'ATIVA A SER AJUIZADA'.
-Você tem os processos 90.2.24.006707-39, 90.2.24.017595-04, 90.4.23.059449-29, 90.4.23.065843-14, 90.4.23.065844-03, 90.4.23.065845-86, 90.4.23.065846-67, 90.4.23.065847-48, 90.4.23.065848-29, 90.4.23.065849-00, 90.4.23.065850-43, 90.4.23.231741-02, 90.4.23.231742-93, 90.4.23.231743-74, 90.4.23.231744-55, 90.4.23.231745-36, 90.4.23.231746-17, 90.4.24.108611-67, 90.4.24.108612-48, 90.4.24.192989-02, 90.4.24.192990-38, 90.5.22.011269-84, 90.5.22.011270-18, 90.5.22.011271-07, 90.5.22.011272-80, 90.5.22.011273-60, 90.5.22.011274-41, 90.5.22.011275-22 em 'ATIVA EM COBRANCA'.</t>
+A empresa possui os seguintes débitos referente a parcelamentos: 
+000520 - INSCRICAO DE CREDITO EM DIVIDA ATIVA'.
+000797 - PARCELAMENTO RESCINDIDO'.
+ATIVA A SER AJUIZADA'.
+ATIVA EM COBRANCA'.
+Os valores informados são válidos na data de envio deste e-mail (03/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>11192559000187</t>
-        </is>
+      <c r="A4" t="n">
+        <v>11192559000187</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HOSPI BIO INDUSTRIA E COMERCIO DE MOVEIS HOSPITALARES LTDA, segue resumo dos seus débitos de FGTS: 12/2024: R$ 3257.15, 13/2024: R$ 1516.12.</t>
+          <t>HOSPI BIO INDUSTRIA E COMERCIO DE MOVEIS HOSPITALARES LTDA, segue resumo dos seus débitos de FGTS: 12/2024: R$ 3257.15, 13/2024: R$ 1516.12.
+Os valores informados são válidos na data de envio deste e-mail (03/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
digitaliza falhando qnd empresa n tem a msg
</commit_message>
<xml_diff>
--- a/mensagens.xlsx
+++ b/mensagens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hdlogika\k\Backup_19_08_2021\Unidade_D\K\LEATICIA\Luiz Fernando\Automation_rfb\d-bitos_rfb_pr-mor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B2CD0C-C164-4C44-A6E0-F4C159426509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF5C753-E607-4889-AEA5-C7A71ED5EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Empresa</t>
   </si>
@@ -28,26 +28,224 @@
     <t>Mensagem</t>
   </si>
   <si>
-    <t>Olá GARCIA &amp; MARQUES M G LTDA,
+    <t>Olá F A BOLOGNESE LTDA,
 Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
 Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
 Segue o resumo dos seus débitos:
 **Referente a 11/2024:**
-  - Departamento Pessoal: R$ 392.69
-Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
-Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
-Ficamos à disposição para qualquer dúvida ou informação adicional!
-Atenciosamente,
-Prímor Contábil
-(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
-  </si>
-  <si>
-    <t>Olá GARCIA MADRUGA LTDA,
-Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
-Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
-Segue o resumo dos seus débitos:
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá BORGHI E NECKEL REPRESENTACOES LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 02/2020:**
+  - outros (PIS): R$ 36.73
+**Referente a 03/2020:**
+  - outros (PIS): R$ 41.98
+**Referente a 07/2024:**
+  - Departamento Pessoal: R$ 544.90
+A empresa possui os seguintes débitos referente a parcelamentos: 
+000520 - INSCRICAO DE CREDITO EM DIVIDA ATIVA'.
+000551 - SIDAT - BLOQUEADO PARA COBRANCA'.
+ATIVA EM COBRANCA'.
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá ADEMIL CONSTRUCOES LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 06/2024:**
+  - outros (PIS): R$ 336.54
+**Referente a 07/2024:**
+  - outros (PIS): R$ 438.53
+**Referente a 08/2024:**
+  - outros (PIS): R$ 892.82
+**Referente a 09/2024:**
+  - outros (PIS): R$ 398.63
+**Referente a 10/2024:**
+  - outros (PIS): R$ 352.40
 **Referente a 11/2024:**
-  - Departamento Pessoal: R$ 734.62
+  - outros (PIS): R$ 148.60
+  - outros (COFINS): R$ 685.89
+A empresa possui os seguintes débitos referente a parcelamentos: 
+000797 - PARCELAMENTO RESCINDIDO'.
+ATIVA A SER AJUIZADA'.
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá A E COLCHOES MOVEIS E ESTOFADOS LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 01/2023:**
+  - Departamento Pessoal: R$ 168.34
+**Referente a 02/2023:**
+  - Departamento Pessoal: R$ 100.06
+**Referente a 04/2024:**
+  - outros (PIS): R$ 128.04
+  - outros (COFINS): R$ 590.98
+**Referente a 05/2024:**
+  - outros (PIS): R$ 216.57
+  - outros (COFINS): R$ 999.56
+  - Departamento Pessoal: R$ 552.69
+**Referente a 06/2024:**
+  - Departamento Pessoal: R$ 548.71
+**Referente a 07/2024:**
+  - outros (PIS): R$ 471.73
+  - Departamento Pessoal: R$ 544.90
+**Referente a 08/2024:**
+  - outros (PIS): R$ 81.89
+  - outros (COFINS): R$ 377.99
+  - Departamento Pessoal: R$ 541.22
+**Referente a 09/2024:**
+  - outros (PIS): R$ 23.53
+  - outros (COFINS): R$ 108.60
+  - Departamento Pessoal: R$ 537.16
+**Referente a 10/2024:**
+  - Departamento Pessoal: R$ 533.70
+**Referente a 11/2024:**
+  - outros (PIS): R$ 35.93
+  - outros (COFINS): R$ 165.85
+  - Departamento Pessoal: R$ 488.31
+A empresa possui os seguintes débitos referente a parcelamentos: 
+000797 - PARCELAMENTO RESCINDIDO'.
+ATIVA EM COBRANCA'.
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá DE ARAUJO TRANSPORTES LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 2024:**
+  - Departamento Pessoal: R$ 258.14
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá A CRUZ DA SILVA COLCHOES E ESTOFADOS,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 08/2024:**
+  - Departamento Pessoal: R$ 644.04
+**Referente a 09/2024:**
+  - Departamento Pessoal: R$ 383.36
+**Referente a 10/2024:**
+  - Departamento Pessoal: R$ 529.49
+**Referente a 11/2024:**
+  - Departamento Pessoal: R$ 529.65
+**Referente a 12/2024:**
+  - Departamento Pessoal: R$ 543.07
+**Referente a 2024:**
+  - Departamento Pessoal: R$ 99.60
+A empresa possui os seguintes débitos referente a parcelamentos: 
+ATIVA NAO AJUIZAVEL EM PROCESSO DE NEGOCIACAO NO SISPAR'.
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá C R V ESTERO E CIA LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 11/2024:**
+  - Departamento Pessoal: R$ 830.31
+A empresa C R V ESTERO E CIA LTDA possui os seguintes débitos referentes a Processos SIEF:
+10950.918.354/2024-11, 10950.917.607/2024-21, 10950.917.603/2024-42, 10950.917.601/2024-53
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá CHARLEN APARECIDO DO VALE FERNANDES CORRETORA DE SEGUROS,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 10/2024:**
+  - outros (SIMPLES NAC.): R$ 758.32
+**Referente a 11/2024:**
+  - outros (SIMPLES NAC.): R$ 700.05
+  - Departamento Pessoal: R$ 173.27
+Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
+Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
+Ficamos à disposição para qualquer dúvida ou informação adicional!
+Atenciosamente,
+Prímor Contábil
+(44) 98462-9927 / atendimento@contabilprimor.com.br</t>
+  </si>
+  <si>
+    <t>Olá AF SOLUCOES EM ENGENHARIA MECANICA LTDA,
+Identificamos que sua empresa possui algumas pendências em aberto junto à Receita Federal.
+Essas pendências podem gerar multas, juros e complicações mais sérias se não forem regularizadas em tempo hábil.
+Segue o resumo dos seus débitos:
+**Referente a 01/2023:**
+  - outros (MAED - PGDAS-D): R$ 89.05
+**Referente a 02/2022:**
+  - outros (SIMPLES NAC.): R$ 189.69
+**Referente a 02/2023:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+**Referente a 03/2023:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+**Referente a 04/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 93.70
+**Referente a 05/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 186.12
+**Referente a 06/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 92.43
+**Referente a 07/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 91.71
+**Referente a 08/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 887.72
+**Referente a 09/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+  - outros (SIMPLES NAC.): R$ 491.61
+**Referente a 10/2022:**
+  - outros (MAED - PGDAS-D): R$ 54.25
+**Referente a 11/2022:**
+  - outros (MAED - PGDAS-D): R$ 50.00
+**Referente a 12/2022:**
+  - outros (MAED - PGDAS-D): R$ 110.05
+  - outros (SIMPLES NAC.): R$ 88.39
 Os valores informados são válidos na data de envio deste e-mail (07/02/25) e podem sofrer alterações.
 Caso tenha interesse em regularizar essas pendências, entre em contato com o nosso time para mais detalhes e orientações sobre os próximos passos.
 Ficamos à disposição para qualquer dúvida ou informação adicional!
@@ -416,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +636,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>44719717000163</v>
+        <v>5087518000128</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -446,10 +644,66 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>51465799000122</v>
+        <v>8325066000163</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11279829000191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14952655000174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15219621000138</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20119119000195</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>23098061000139</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>24269050000137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>29813455000108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>